<commit_message>
Add review checklist testcase
</commit_message>
<xml_diff>
--- a/project/templates/Compatibility test_case.xlsx
+++ b/project/templates/Compatibility test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongnhat/Desktop/Project-KTPM/project/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE3B4C0-AC7D-4243-A283-CF8AFB9ED549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D297A17-AA67-0B49-9587-8015837E982F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20060" tabRatio="821" activeTab="5" xr2:uid="{54D1C333-A8F3-504F-8D67-28F9DF72E520}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20060" tabRatio="821" activeTab="2" xr2:uid="{54D1C333-A8F3-504F-8D67-28F9DF72E520}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="174">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -639,9 +639,6 @@
   </si>
   <si>
     <t>UI reference data for OS compatibility</t>
-  </si>
-  <si>
-    <t>Font, color, icons consistent</t>
   </si>
   <si>
     <t>Product: Burger; Detail: Ngon</t>
@@ -2425,7 +2422,7 @@
       <c r="B11" s="48"/>
       <c r="C11" s="49"/>
       <c r="D11" s="101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="50"/>
       <c r="F11" s="51"/>
@@ -2526,9 +2523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D16ABC5-B443-FF41-BA73-04E67E6728A8}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2957,7 +2954,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="C9:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -3347,7 +3344,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -3364,7 +3361,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="117" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="114" t="s">
         <v>145</v>
@@ -3381,7 +3378,7 @@
     </row>
     <row r="2" spans="1:5" ht="18">
       <c r="A2" s="133" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="115" t="s">
         <v>57</v>
@@ -3390,7 +3387,7 @@
         <v>148</v>
       </c>
       <c r="D2" s="115" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" s="115" t="s">
         <v>93</v>
@@ -3405,7 +3402,7 @@
         <v>148</v>
       </c>
       <c r="D3" s="115" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E3" s="115" t="s">
         <v>94</v>
@@ -3420,7 +3417,7 @@
         <v>148</v>
       </c>
       <c r="D4" s="115" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E4" s="115" t="s">
         <v>95</v>
@@ -3435,7 +3432,7 @@
         <v>149</v>
       </c>
       <c r="D5" s="116" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="115" t="s">
         <v>96</v>
@@ -3450,7 +3447,7 @@
         <v>150</v>
       </c>
       <c r="D6" s="115" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="115" t="s">
         <v>97</v>
@@ -3465,7 +3462,7 @@
         <v>151</v>
       </c>
       <c r="D7" s="115" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" s="115" t="s">
         <v>98</v>
@@ -3480,7 +3477,7 @@
         <v>152</v>
       </c>
       <c r="D8" s="115" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E8" s="115" t="s">
         <v>99</v>
@@ -3488,7 +3485,7 @@
     </row>
     <row r="9" spans="1:5" ht="18">
       <c r="A9" s="133" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="115" t="s">
         <v>64</v>
@@ -3497,7 +3494,7 @@
         <v>153</v>
       </c>
       <c r="D9" s="115" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" s="115" t="s">
         <v>110</v>
@@ -3512,7 +3509,7 @@
         <v>154</v>
       </c>
       <c r="D10" s="115" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" s="115" t="s">
         <v>111</v>
@@ -3527,7 +3524,7 @@
         <v>155</v>
       </c>
       <c r="D11" s="116" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" s="115" t="s">
         <v>112</v>
@@ -3542,7 +3539,7 @@
         <v>156</v>
       </c>
       <c r="D12" s="115" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E12" s="115" t="s">
         <v>113</v>
@@ -3557,7 +3554,7 @@
         <v>158</v>
       </c>
       <c r="D13" s="115" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E13" s="115" t="s">
         <v>114</v>
@@ -3572,7 +3569,7 @@
         <v>160</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E14" s="115" t="s">
         <v>115</v>
@@ -3592,7 +3589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64336199-8AF6-B940-8B43-002AEC695EDA}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I27:I28"/>
     </sheetView>
   </sheetViews>
@@ -3883,15 +3880,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005EA2A741C5885C41AB9A358CCBEA8A85" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b08c537a49adf1f0264621696145d4e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="41A7A25E-88C5-415C-AB9A-358CCBEA8A85" xmlns:ns3="cd6d2771-e08b-42a3-90f8-eca630337659" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79edc66073723f43766a972d30b274e4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4265,15 +4253,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85ED280E-F51D-42B1-B363-4EC477D089ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCAE63D-5380-40ED-A43E-1567E1C20371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4290,4 +4279,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85ED280E-F51D-42B1-B363-4EC477D089ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>